<commit_message>
Se agrega pruebas ejemplo
</commit_message>
<xml_diff>
--- a/BaseWebUI/src/test/resources/datadriven/BaseDataDriven.xlsx
+++ b/BaseWebUI/src/test/resources/datadriven/BaseDataDriven.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/jsanchbe_emeal_nttdata_com/Documents/Escritorio/Ecopetrol/Devops/BaseAutomation/BaseWebUI/src/test/resources/datadriven/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{DF29B8EF-655B-479F-BC5A-EF8C74A3648E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{377319EC-1490-4D70-A1B9-F5440016AFEC}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{DF29B8EF-655B-479F-BC5A-EF8C74A3648E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80CEBB21-6F19-479F-9AC4-3FEC8CE8D8BA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exitoso" sheetId="7" r:id="rId1"/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="155">
   <si>
     <t>Caso</t>
   </si>
@@ -557,13 +557,16 @@
     <t>visual_user</t>
   </si>
   <si>
-    <t>other_user</t>
-  </si>
-  <si>
     <t>AssertText</t>
   </si>
   <si>
     <t>Products</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Epic sadface: Username and password do not match any user in this service</t>
   </si>
 </sst>
 </file>
@@ -951,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5483BD97-5A7B-4372-AD24-B7F7EBCD439D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -972,7 +975,7 @@
         <v>147</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -986,7 +989,7 @@
         <v>149</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1000,7 +1003,7 @@
         <v>149</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1016,15 +1019,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F6A408-94AD-4CCD-942B-E296704F3D24}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1034,16 +1037,22 @@
       <c r="C1" s="5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>149</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1868,6 +1877,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c5abdf2c-8a16-4886-be54-ed4e62a70697">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009263D68DC986354AA92EC9047B5038EB" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f0fc7e6aef46ec809f6e445356902ed4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c5abdf2c-8a16-4886-be54-ed4e62a70697" xmlns:ns3="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfe9d55b7a83ace495aa0670d0536b79" ns2:_="" ns3:_="">
     <xsd:import namespace="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
@@ -2070,17 +2090,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c5abdf2c-8a16-4886-be54-ed4e62a70697">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2091,6 +2100,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABF929D3-10AB-4E3C-8DD6-925C7C3F2BB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
+    <ds:schemaRef ds:uri="6dcff6fb-c744-4b82-8f0b-4ce71711ce53"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BAEAE49-7210-4672-A178-C5B35DBE9EC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2109,17 +2129,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABF929D3-10AB-4E3C-8DD6-925C7C3F2BB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
-    <ds:schemaRef ds:uri="6dcff6fb-c744-4b82-8f0b-4ce71711ce53"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C92B58EC-22A6-4E3C-8F79-6DC894C45947}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Se agrega ejemplo exitoso y fallido
</commit_message>
<xml_diff>
--- a/BaseWebUI/src/test/resources/datadriven/BaseDataDriven.xlsx
+++ b/BaseWebUI/src/test/resources/datadriven/BaseDataDriven.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/jsanchbe_emeal_nttdata_com/Documents/Escritorio/Ecopetrol/Devops/BaseAutomation/BaseWebUI/src/test/resources/datadriven/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{DF29B8EF-655B-479F-BC5A-EF8C74A3648E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80CEBB21-6F19-479F-9AC4-3FEC8CE8D8BA}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{DF29B8EF-655B-479F-BC5A-EF8C74A3648E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B5E784B-FCA7-4D29-AB88-523563AFF406}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exitoso" sheetId="7" r:id="rId1"/>
@@ -954,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5483BD97-5A7B-4372-AD24-B7F7EBCD439D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,11 +1021,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F6A408-94AD-4CCD-942B-E296704F3D24}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
@@ -1877,17 +1880,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c5abdf2c-8a16-4886-be54-ed4e62a70697">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009263D68DC986354AA92EC9047B5038EB" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f0fc7e6aef46ec809f6e445356902ed4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c5abdf2c-8a16-4886-be54-ed4e62a70697" xmlns:ns3="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfe9d55b7a83ace495aa0670d0536b79" ns2:_="" ns3:_="">
     <xsd:import namespace="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
@@ -2090,6 +2082,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c5abdf2c-8a16-4886-be54-ed4e62a70697">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2100,17 +2103,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABF929D3-10AB-4E3C-8DD6-925C7C3F2BB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
-    <ds:schemaRef ds:uri="6dcff6fb-c744-4b82-8f0b-4ce71711ce53"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BAEAE49-7210-4672-A178-C5B35DBE9EC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2129,6 +2121,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABF929D3-10AB-4E3C-8DD6-925C7C3F2BB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
+    <ds:schemaRef ds:uri="6dcff6fb-c744-4b82-8f0b-4ce71711ce53"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C92B58EC-22A6-4E3C-8F79-6DC894C45947}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Complemento de test base
</commit_message>
<xml_diff>
--- a/BaseWebUI/src/test/resources/datadriven/BaseDataDriven.xlsx
+++ b/BaseWebUI/src/test/resources/datadriven/BaseDataDriven.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{DF29B8EF-655B-479F-BC5A-EF8C74A3648E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B5E784B-FCA7-4D29-AB88-523563AFF406}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exitoso" sheetId="7" r:id="rId1"/>
@@ -954,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5483BD97-5A7B-4372-AD24-B7F7EBCD439D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F6A408-94AD-4CCD-942B-E296704F3D24}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1880,6 +1880,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c5abdf2c-8a16-4886-be54-ed4e62a70697">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009263D68DC986354AA92EC9047B5038EB" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f0fc7e6aef46ec809f6e445356902ed4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c5abdf2c-8a16-4886-be54-ed4e62a70697" xmlns:ns3="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfe9d55b7a83ace495aa0670d0536b79" ns2:_="" ns3:_="">
     <xsd:import namespace="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
@@ -2082,17 +2093,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c5abdf2c-8a16-4886-be54-ed4e62a70697">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2103,6 +2103,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABF929D3-10AB-4E3C-8DD6-925C7C3F2BB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
+    <ds:schemaRef ds:uri="6dcff6fb-c744-4b82-8f0b-4ce71711ce53"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BAEAE49-7210-4672-A178-C5B35DBE9EC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2121,17 +2132,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABF929D3-10AB-4E3C-8DD6-925C7C3F2BB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
-    <ds:schemaRef ds:uri="6dcff6fb-c744-4b82-8f0b-4ce71711ce53"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C92B58EC-22A6-4E3C-8F79-6DC894C45947}">
   <ds:schemaRefs>

</xml_diff>